<commit_message>
added poision sumac to the list of shrubs
</commit_message>
<xml_diff>
--- a/output/ESIS.table.compare.xlsx
+++ b/output/ESIS.table.compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace2\match_pedon_site\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F935BFB-FC70-4C02-ADE5-6826848B9B60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740EA14A-F7D8-4297-AB46-82A4C3B3E083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1045,10 +1045,10 @@
   <dimension ref="A1:U58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3:U58"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,7 +1921,7 @@
         <v>1.5</v>
       </c>
       <c r="F17" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G17" s="1">
         <v>0.2</v>
@@ -1939,16 +1939,16 @@
         <v>11</v>
       </c>
       <c r="N17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="O17" s="7">
         <v>0.2</v>
       </c>
-      <c r="O17" s="7">
-        <v>0.5</v>
-      </c>
       <c r="P17" s="1">
         <v>1</v>
       </c>
       <c r="Q17" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R17" s="1">
         <v>0.1</v>
@@ -1998,10 +1998,10 @@
         <v>12</v>
       </c>
       <c r="N18" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="O18" s="8">
         <v>0.2</v>
-      </c>
-      <c r="O18" s="8">
-        <v>0.4</v>
       </c>
       <c r="P18" s="3">
         <v>1</v>
@@ -2039,7 +2039,7 @@
         <v>10</v>
       </c>
       <c r="F19" s="8">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G19" s="3">
         <v>2</v>
@@ -2057,16 +2057,16 @@
         <v>13</v>
       </c>
       <c r="N19" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="O19" s="8">
         <v>0.2</v>
-      </c>
-      <c r="O19" s="8">
-        <v>0.5</v>
       </c>
       <c r="P19" s="3">
         <v>10</v>
       </c>
       <c r="Q19" s="8">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="R19" s="3">
         <v>0.5</v>
@@ -2089,16 +2089,16 @@
         <v>14</v>
       </c>
       <c r="C20" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D20" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E20" s="3">
         <v>10</v>
       </c>
       <c r="F20" s="8">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G20" s="3">
         <v>1</v>
@@ -2116,16 +2116,16 @@
         <v>14</v>
       </c>
       <c r="N20" s="3">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="O20" s="8">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="P20" s="3">
         <v>10</v>
       </c>
       <c r="Q20" s="8">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="R20" s="3">
         <v>3</v>
@@ -2148,7 +2148,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="3">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D21" s="8">
         <v>45</v>
@@ -2157,7 +2157,7 @@
         <v>10</v>
       </c>
       <c r="F21" s="8">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G21" s="3">
         <v>0</v>
@@ -2175,16 +2175,16 @@
         <v>15</v>
       </c>
       <c r="N21" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O21" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="P21" s="3">
         <v>10</v>
       </c>
       <c r="Q21" s="8">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="R21" s="3">
         <v>0.4</v>
@@ -2597,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="8">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="8"/>
@@ -2612,8 +2612,12 @@
       <c r="O29" s="8">
         <v>20</v>
       </c>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="8"/>
+      <c r="P29" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Q29" s="8">
+        <v>0.5</v>
+      </c>
       <c r="R29" s="3"/>
       <c r="S29" s="8"/>
       <c r="T29" s="3"/>
@@ -2651,8 +2655,12 @@
       <c r="O30" s="9">
         <v>4</v>
       </c>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="9"/>
+      <c r="P30" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="9">
+        <v>0</v>
+      </c>
       <c r="R30" s="5"/>
       <c r="S30" s="9"/>
       <c r="T30" s="5"/>
@@ -3030,7 +3038,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -3057,13 +3065,13 @@
         <v>0</v>
       </c>
       <c r="O38" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P38" s="1">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="Q38" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="R38" s="1">
         <v>20</v>
@@ -3089,7 +3097,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
@@ -3116,13 +3124,13 @@
         <v>0</v>
       </c>
       <c r="O39" s="8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P39" s="3">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="Q39" s="8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="R39" s="3">
         <v>20</v>
@@ -3148,10 +3156,10 @@
         <v>0</v>
       </c>
       <c r="D40" s="8">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3">
         <v>0.1</v>
-      </c>
-      <c r="E40" s="3">
-        <v>0</v>
       </c>
       <c r="F40" s="8">
         <v>20</v>
@@ -3175,10 +3183,10 @@
         <v>0</v>
       </c>
       <c r="O40" s="8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P40" s="3">
-        <v>10</v>
+        <v>1.5</v>
       </c>
       <c r="Q40" s="8">
         <v>25</v>
@@ -3207,7 +3215,7 @@
         <v>0</v>
       </c>
       <c r="D41" s="8">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
@@ -3234,10 +3242,10 @@
         <v>0.2</v>
       </c>
       <c r="O41" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P41" s="3">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="Q41" s="8">
         <v>20</v>
@@ -3266,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="D42" s="8">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="E42" s="3">
         <v>0</v>
@@ -3293,10 +3301,10 @@
         <v>0.2</v>
       </c>
       <c r="O42" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P42" s="3">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="Q42" s="8">
         <v>20</v>
@@ -3790,7 +3798,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G52" s="1">
         <v>0</v>
@@ -3811,7 +3819,7 @@
         <v>0.2</v>
       </c>
       <c r="O52" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P52" s="1">
         <v>0</v>
@@ -3849,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="8">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G53" s="3">
         <v>0</v>
@@ -3870,13 +3878,13 @@
         <v>0.2</v>
       </c>
       <c r="O53" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P53" s="3">
         <v>0</v>
       </c>
       <c r="Q53" s="8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R53" s="3">
         <v>0.4</v>
@@ -3929,7 +3937,7 @@
         <v>0.2</v>
       </c>
       <c r="O54" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P54" s="3">
         <v>0.1</v>
@@ -3988,7 +3996,7 @@
         <v>0</v>
       </c>
       <c r="O55" s="8">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="P55" s="3">
         <v>0.1</v>

</xml_diff>